<commit_message>
updaten pin and splash
</commit_message>
<xml_diff>
--- a/server/data.xlsx
+++ b/server/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>Dari Jam</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Real Budget</t>
   </si>
   <si>
-    <t>Column 1</t>
+    <t>PIC</t>
   </si>
   <si>
     <t>Keterangan</t>
@@ -49,21 +49,12 @@
     <t>Wait and prepare to flight</t>
   </si>
   <si>
-    <t>Rp-</t>
-  </si>
-  <si>
     <t>Tunggu keberangkatan pesawat</t>
   </si>
   <si>
     <t>Flight to Singapore</t>
   </si>
   <si>
-    <t>Rp1,250,000</t>
-  </si>
-  <si>
-    <t>Rp1,116,221</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -88,12 +79,6 @@
     <t>Check in Hotel, beres-beres, sholat maghrib</t>
   </si>
   <si>
-    <t>Rp1,850,000</t>
-  </si>
-  <si>
-    <t>Rp1,830,127</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -241,9 +226,6 @@
     <t>Bus SG to KL (Berjaya Times Square)</t>
   </si>
   <si>
-    <t>Rp1,000,000</t>
-  </si>
-  <si>
     <t>2 Pax, Qistna Express</t>
   </si>
   <si>
@@ -377,12 +359,6 @@
   </si>
   <si>
     <t>Flight to Jakarta</t>
-  </si>
-  <si>
-    <t>Rp1,700,000</t>
-  </si>
-  <si>
-    <t>Rp1,749,145</t>
   </si>
   <si>
     <t>KLM Royal Dutch Airlines</t>
@@ -397,7 +373,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy h:mm"/>
-    <numFmt numFmtId="165" formatCode="&quot;Rp&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;(#,##0.00)"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -552,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -580,6 +556,12 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -590,7 +572,19 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -603,6 +597,12 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,7 +662,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I70" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I70" displayName="Activities" name="Activities" id="1">
   <tableColumns count="9">
     <tableColumn name="Dari Jam" id="1"/>
     <tableColumn name="Sampai Jam" id="2"/>
@@ -670,7 +670,7 @@
     <tableColumn name="Kegiatan" id="4"/>
     <tableColumn name="Estimasi Biaya" id="5"/>
     <tableColumn name="Real Budget" id="6"/>
-    <tableColumn name="Column 1" id="7"/>
+    <tableColumn name="PIC" id="7"/>
     <tableColumn name="Keterangan" id="8"/>
     <tableColumn name="Column 2" id="9"/>
   </tableColumns>
@@ -888,8 +888,8 @@
     <col customWidth="1" min="1" max="1" width="15.38"/>
     <col customWidth="1" min="2" max="2" width="14.75"/>
     <col customWidth="1" min="4" max="4" width="34.25"/>
-    <col customWidth="1" min="5" max="5" width="16.38"/>
-    <col customWidth="1" min="6" max="6" width="14.38"/>
+    <col customWidth="1" min="5" max="5" width="19.63"/>
+    <col customWidth="1" min="6" max="6" width="17.63"/>
     <col customWidth="1" min="8" max="8" width="37.63"/>
     <col customWidth="1" min="9" max="9" width="2.38"/>
   </cols>
@@ -937,30 +937,32 @@
         <v>9</v>
       </c>
       <c r="E2" s="8">
-        <v>150.0</v>
-      </c>
+        <v>140000.0</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>45862.354166666664</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>45862.46527777778</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="13">
         <v>160.0</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -974,37 +976,37 @@
         <v>170.0</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1250000.0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1116221.0</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="11">
+        <v>45862.583333333336</v>
+      </c>
+      <c r="B5" s="12">
+        <v>45862.59375</v>
+      </c>
+      <c r="C5" s="13">
+        <v>15.0</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9">
-        <v>45862.583333333336</v>
-      </c>
-      <c r="B5" s="10">
-        <v>45862.59375</v>
-      </c>
-      <c r="C5" s="11">
-        <v>15.0</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6">
       <c r="A6" s="5">
@@ -1017,33 +1019,35 @@
         <v>60.0</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="11">
+        <v>45862.635416666664</v>
+      </c>
+      <c r="B7" s="12">
+        <v>45862.677083333336</v>
+      </c>
+      <c r="C7" s="13">
+        <v>60.0</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="17">
+        <v>50000.0</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="13" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9">
-        <v>45862.635416666664</v>
-      </c>
-      <c r="B7" s="10">
-        <v>45862.677083333336</v>
-      </c>
-      <c r="C7" s="11">
-        <v>60.0</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="12">
-        <v>50.0</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -1057,39 +1061,41 @@
         <v>135.0</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1850000.0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1830127.0</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11">
+        <v>45862.770833333336</v>
+      </c>
+      <c r="B9" s="12">
+        <v>45862.79861111111</v>
+      </c>
+      <c r="C9" s="13">
+        <v>40.0</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E9" s="17">
+        <v>50000.0</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9">
-        <v>45862.770833333336</v>
-      </c>
-      <c r="B9" s="10">
-        <v>45862.79861111111</v>
-      </c>
-      <c r="C9" s="11">
-        <v>40.0</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="12">
-        <v>50.0</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -1103,33 +1109,35 @@
         <v>50.0</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E10" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9">
+      <c r="A11" s="11">
         <v>45862.833333333336</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="12">
         <v>45862.84027777778</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="13">
         <v>10.0</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>34</v>
+      <c r="D11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -1143,33 +1151,37 @@
         <v>80.0</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E12" s="8">
-        <v>500.0</v>
-      </c>
+        <v>500000.0</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9">
+      <c r="A13" s="11">
         <v>45862.895833333336</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="12">
         <v>45862.9375</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="13">
         <v>60.0</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="12">
-        <v>60.0</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>38</v>
+      <c r="D13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="17">
+        <v>60000.0</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -1177,28 +1189,33 @@
         <v>45862.9375</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9">
+      <c r="A15" s="11">
         <v>45863.3125</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="12">
         <v>45863.354166666664</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="13">
         <v>60.0</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="12">
-        <v>120.0</v>
-      </c>
+      <c r="D15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="17">
+        <v>120000.0</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16">
       <c r="A16" s="5">
@@ -1211,33 +1228,37 @@
         <v>75.0</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E16" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>45863.40625</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="12">
         <v>45863.447916666664</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="13">
         <v>60.0</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="12">
-        <v>100.0</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>45</v>
+      <c r="D17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18">
@@ -1251,33 +1272,33 @@
         <v>20.0</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9">
+      <c r="A19" s="11">
         <v>45863.461805555555</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="12">
         <v>45863.50347222222</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="13">
         <v>60.0</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>45</v>
+      <c r="D19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="20">
@@ -1291,33 +1312,37 @@
         <v>25.0</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E20" s="8">
-        <v>50.0</v>
-      </c>
+        <v>50000.0</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9">
+      <c r="A21" s="11">
         <v>45863.520833333336</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="12">
         <v>45863.604166666664</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="13">
         <v>120.0</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="12">
-        <v>150.0</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>52</v>
+      <c r="D21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="17">
+        <v>150000.0</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22">
@@ -1331,31 +1356,35 @@
         <v>40.0</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E22" s="8">
-        <v>50.0</v>
-      </c>
+        <v>50000.0</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="9">
+      <c r="A23" s="11">
         <v>45863.631944444445</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="12">
         <v>45863.663194444445</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="13">
         <v>45.0</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="17">
         <v>100.0</v>
       </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24">
       <c r="A24" s="5">
@@ -1368,33 +1397,37 @@
         <v>30.0</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E24" s="8">
-        <v>50.0</v>
-      </c>
+        <v>50000.0</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="9">
+      <c r="A25" s="11">
         <v>45863.68402777778</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="12">
         <v>45863.725694444445</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="13">
         <v>60.0</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="12">
-        <v>500.0</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>59</v>
+      <c r="D25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="17">
+        <v>500000.0</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26">
@@ -1408,31 +1441,35 @@
         <v>45.0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E26" s="8">
-        <v>50.0</v>
-      </c>
+        <v>50000.0</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="9">
+      <c r="A27" s="11">
         <v>45863.756944444445</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="12">
         <v>45863.79861111111</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="13">
         <v>60.0</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="12">
-        <v>100.0</v>
-      </c>
+      <c r="D27" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28">
       <c r="A28" s="5">
@@ -1445,33 +1482,37 @@
         <v>30.0</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E28" s="8">
-        <v>40.0</v>
-      </c>
+        <v>40000.0</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
         <v>45863.819444444445</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="12">
         <v>45863.86111111111</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="13">
         <v>60.0</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="12">
-        <v>250.0</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>66</v>
+      <c r="D29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="17">
+        <v>250000.0</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30">
@@ -1485,58 +1526,66 @@
         <v>30.0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E30" s="8">
-        <v>40.0</v>
-      </c>
+        <v>40000.0</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="9">
+      <c r="A31" s="11">
         <v>45863.881944444445</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="12">
         <v>45863.92361111111</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="13">
         <v>60.0</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>68</v>
-      </c>
+      <c r="D31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32">
       <c r="A32" s="5">
         <v>45863.92361111111</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="9">
+      <c r="A33" s="11">
         <v>45864.3125</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="12">
         <v>45864.322916666664</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="13">
         <v>15.0</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>70</v>
+      <c r="D33" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="34">
@@ -1550,31 +1599,35 @@
         <v>20.0</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E34" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="9">
+      <c r="A35" s="11">
         <v>45864.336805555555</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="12">
         <v>45864.354166666664</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="13">
         <v>25.0</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="12">
-        <v>130.0</v>
-      </c>
+      <c r="D35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="17">
+        <v>130000.0</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
     </row>
     <row r="36">
       <c r="A36" s="5">
@@ -1587,36 +1640,36 @@
         <v>30.0</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37">
-      <c r="A37" s="9">
+      <c r="A37" s="11">
         <v>45864.375</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="12">
         <v>45864.625</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="13">
         <v>360.0</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F37" s="12">
-        <v>815.0</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>77</v>
+      <c r="D37" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="17">
+        <v>1000000.0</v>
+      </c>
+      <c r="F37" s="17">
+        <v>815000.0</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="38">
@@ -1630,36 +1683,36 @@
         <v>40.0</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39">
-      <c r="A39" s="9">
+      <c r="A39" s="11">
         <v>45864.65277777778</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="12">
         <v>45864.663194444445</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="13">
         <v>15.0</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="12">
-        <v>800.0</v>
-      </c>
-      <c r="F39" s="12">
-        <v>805.805</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>80</v>
+      <c r="D39" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="17">
+        <v>800000.0</v>
+      </c>
+      <c r="F39" s="17">
+        <v>805805.0</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="40">
@@ -1673,28 +1726,28 @@
         <v>130.0</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41">
-      <c r="A41" s="9">
+      <c r="A41" s="11">
         <v>45864.75347222222</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="12">
         <v>45864.76388888889</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="13">
         <v>15.0</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="D41" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="15"/>
     </row>
     <row r="42">
       <c r="A42" s="5">
@@ -1707,33 +1760,37 @@
         <v>60.0</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E42" s="8">
-        <v>120.0</v>
-      </c>
+        <v>120000.0</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="10"/>
       <c r="H42" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="9">
+      <c r="A43" s="11">
         <v>45864.805555555555</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="12">
         <v>45864.81597222222</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="13">
         <v>15.0</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="12">
-        <v>30.0</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>86</v>
+      <c r="D43" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="17">
+        <v>30000.0</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="44">
@@ -1747,33 +1804,37 @@
         <v>15.0</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E44" s="8">
-        <v>30.0</v>
-      </c>
+        <v>30000.0</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="10"/>
       <c r="H44" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="9">
+      <c r="A45" s="11">
         <v>45864.82638888889</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="12">
         <v>45864.868055555555</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="13">
         <v>60.0</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="12">
-        <v>100.0</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>90</v>
+      <c r="D45" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F45" s="14"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="46">
@@ -1787,24 +1848,26 @@
         <v>10.0</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E46" s="8">
-        <v>70.0</v>
-      </c>
+        <v>70000.0</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47">
-      <c r="A47" s="9">
+      <c r="A47" s="11">
         <v>45864.875</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>40</v>
+      <c r="D47" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="48">
@@ -1818,28 +1881,30 @@
         <v>60.0</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E48" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49">
-      <c r="A49" s="9">
+      <c r="A49" s="11">
         <v>45865.375</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="12">
         <v>45865.381944444445</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="13">
         <v>10.0</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="D49" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="15"/>
     </row>
     <row r="50">
       <c r="A50" s="5">
@@ -1852,33 +1917,35 @@
         <v>20.0</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E50" s="8">
-        <v>20.0</v>
-      </c>
+        <v>20000.0</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="10"/>
       <c r="H50" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="9">
+      <c r="A51" s="11">
         <v>45865.395833333336</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="12">
         <v>45865.40277777778</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="13">
         <v>10.0</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E51" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>96</v>
+      <c r="D51" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="52">
@@ -1892,30 +1959,34 @@
         <v>120.0</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E52" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F52" s="9"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53">
-      <c r="A53" s="9">
+      <c r="A53" s="11">
         <v>45865.48611111111</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="12">
         <v>45865.49652777778</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="13">
         <v>15.0</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E53" s="12">
-        <v>150.0</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>99</v>
+      <c r="D53" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="17">
+        <v>150000.0</v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="54">
@@ -1929,33 +2000,35 @@
         <v>90.0</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="10"/>
       <c r="H54" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="9">
+      <c r="A55" s="11">
         <v>45865.55902777778</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="12">
         <v>45865.76736111111</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="13">
         <v>300.0</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E55" s="12">
-        <v>700.0</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>103</v>
+      <c r="D55" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="17">
+        <v>700000.0</v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="56">
@@ -1969,31 +2042,33 @@
         <v>15.0</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="10"/>
       <c r="H56" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="9">
+      <c r="A57" s="11">
         <v>45865.77777777778</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B57" s="12">
         <v>45865.84027777778</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="13">
         <v>90.0</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="E57" s="12">
-        <v>100.0</v>
-      </c>
+      <c r="D57" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
     </row>
     <row r="58">
       <c r="A58" s="5">
@@ -2006,33 +2081,37 @@
         <v>15.0</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E58" s="8">
-        <v>20.0</v>
-      </c>
+        <v>20000.0</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="10"/>
       <c r="H58" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="9">
+      <c r="A59" s="11">
         <v>45865.850694444445</v>
       </c>
-      <c r="B59" s="10">
+      <c r="B59" s="12">
         <v>45865.875</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="13">
         <v>35.0</v>
       </c>
-      <c r="D59" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" s="12">
-        <v>100.0</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>110</v>
+      <c r="D59" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="60">
@@ -2040,33 +2119,35 @@
         <v>45865.875</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="10"/>
       <c r="H60" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="9">
+      <c r="A61" s="11">
         <v>45866.333333333336</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="12">
         <v>45866.395833333336</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="13">
         <v>90.0</v>
       </c>
-      <c r="D61" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E61" s="12">
-        <v>500.0</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>113</v>
+      <c r="D61" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" s="17">
+        <v>500000.0</v>
+      </c>
+      <c r="F61" s="14"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="13" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="62">
@@ -2080,30 +2161,32 @@
         <v>120.0</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="10"/>
     </row>
     <row r="63">
-      <c r="A63" s="9">
+      <c r="A63" s="11">
         <v>45866.479166666664</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="12">
         <v>45866.493055555555</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="13">
         <v>20.0</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E63" s="12">
-        <v>100.0</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>115</v>
+      <c r="D63" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F63" s="14"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="64">
@@ -2117,28 +2200,32 @@
         <v>25.0</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E64" s="8">
-        <v>50.0</v>
-      </c>
+        <v>50000.0</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="10"/>
     </row>
     <row r="65">
-      <c r="A65" s="9">
+      <c r="A65" s="11">
         <v>45866.510416666664</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="12">
         <v>45866.541666666664</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="13">
         <v>45.0</v>
       </c>
-      <c r="D65" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E65" s="12">
-        <v>100.0</v>
-      </c>
+      <c r="D65" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="17">
+        <v>100000.0</v>
+      </c>
+      <c r="F65" s="14"/>
+      <c r="G65" s="15"/>
     </row>
     <row r="66">
       <c r="A66" s="5">
@@ -2151,28 +2238,30 @@
         <v>120.0</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E66" s="8">
-        <v>100.0</v>
-      </c>
+        <v>100000.0</v>
+      </c>
+      <c r="F66" s="9"/>
+      <c r="G66" s="10"/>
     </row>
     <row r="67">
-      <c r="A67" s="9">
+      <c r="A67" s="11">
         <v>45866.625</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="12">
         <v>45866.666666666664</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="13">
         <v>60.0</v>
       </c>
-      <c r="D67" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="D67" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
     </row>
     <row r="68">
       <c r="A68" s="5">
@@ -2185,55 +2274,57 @@
         <v>90.0</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="10"/>
     </row>
     <row r="69">
-      <c r="A69" s="9">
+      <c r="A69" s="11">
         <v>45866.729166666664</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="12">
         <v>45866.8125</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="13">
         <v>120.0</v>
       </c>
-      <c r="D69" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>124</v>
+      <c r="D69" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="17">
+        <v>1700000.0</v>
+      </c>
+      <c r="F69" s="17">
+        <v>1749145.0</v>
+      </c>
+      <c r="G69" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="13">
+      <c r="A70" s="19">
         <v>45866.8125</v>
       </c>
-      <c r="B70" s="14">
+      <c r="B70" s="20">
         <v>45866.916666666664</v>
       </c>
-      <c r="C70" s="15">
+      <c r="C70" s="21">
         <v>150.0</v>
       </c>
-      <c r="D70" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E70" s="16">
-        <v>150.0</v>
-      </c>
-      <c r="H70" s="15" t="s">
+      <c r="D70" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E70" s="22">
+        <v>150000.0</v>
+      </c>
+      <c r="F70" s="23"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2241,6 +2332,9 @@
   <dataValidations>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A70">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="E2:F70">
+      <formula1>AND(ISNUMBER(E2),(NOT(OR(NOT(ISERROR(DATEVALUE(E2))), AND(ISNUMBER(E2), LEFT(CELL("format", E2))="D")))))</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>

</xml_diff>